<commit_message>
added code to perform feature selection. Still needs to be added to main training pipeline.
</commit_message>
<xml_diff>
--- a/AFL_ML/Data/Brisbane_stats.xlsx
+++ b/AFL_ML/Data/Brisbane_stats.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:KV102"/>
+  <dimension ref="A1:KW102"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="HZ1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="IL36" activeCellId="0" sqref="IL36"/>
@@ -1384,8 +1384,11 @@
       <c r="KU1" s="2" t="n">
         <v>10748</v>
       </c>
-      <c r="KV1" t="n">
+      <c r="KV1" s="2" t="n">
         <v>10754</v>
+      </c>
+      <c r="KW1" t="n">
+        <v>10761</v>
       </c>
     </row>
     <row r="2" ht="13.9" customHeight="1" s="3">
@@ -2312,7 +2315,10 @@
       <c r="KU2" s="2" t="n">
         <v>2022</v>
       </c>
-      <c r="KV2" t="n">
+      <c r="KV2" s="2" t="n">
+        <v>2023</v>
+      </c>
+      <c r="KW2" t="n">
         <v>2023</v>
       </c>
     </row>
@@ -3240,8 +3246,11 @@
       <c r="KU3" s="2" t="n">
         <v>27</v>
       </c>
-      <c r="KV3" t="n">
+      <c r="KV3" s="2" t="n">
         <v>1</v>
+      </c>
+      <c r="KW3" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="4" ht="13.9" customHeight="1" s="3">
@@ -4168,8 +4177,11 @@
       <c r="KU4" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="KV4" t="n">
+      <c r="KV4" s="2" t="n">
         <v>1</v>
+      </c>
+      <c r="KW4" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="5" ht="13.9" customHeight="1" s="3">
@@ -5096,7 +5108,10 @@
       <c r="KU5" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="KV5" t="n">
+      <c r="KV5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="KW5" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6024,8 +6039,11 @@
       <c r="KU6" s="2" t="n">
         <v>49</v>
       </c>
-      <c r="KV6" t="n">
+      <c r="KV6" s="2" t="n">
         <v>72</v>
+      </c>
+      <c r="KW6" t="n">
+        <v>93</v>
       </c>
     </row>
     <row r="7" ht="13.9" customHeight="1" s="3">
@@ -6952,8 +6970,11 @@
       <c r="KU7" s="2" t="n">
         <v>120</v>
       </c>
-      <c r="KV7" t="n">
+      <c r="KV7" s="2" t="n">
         <v>126</v>
+      </c>
+      <c r="KW7" t="n">
+        <v>82</v>
       </c>
     </row>
     <row r="8" ht="13.9" customHeight="1" s="3">
@@ -7880,8 +7901,11 @@
       <c r="KU8" s="2" t="n">
         <v>-71</v>
       </c>
-      <c r="KV8" t="n">
+      <c r="KV8" s="2" t="n">
         <v>-54</v>
+      </c>
+      <c r="KW8" t="n">
+        <v>11</v>
       </c>
     </row>
     <row r="9" ht="13.9" customHeight="1" s="3">
@@ -8808,8 +8832,11 @@
       <c r="KU9" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="KV9" t="n">
+      <c r="KV9" s="2" t="n">
         <v>0</v>
+      </c>
+      <c r="KW9" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="10" ht="13.9" customHeight="1" s="3">
@@ -9736,8 +9763,11 @@
       <c r="KU10" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="KV10" t="n">
+      <c r="KV10" s="2" t="n">
         <v>13</v>
+      </c>
+      <c r="KW10" t="n">
+        <v>11</v>
       </c>
     </row>
     <row r="11" ht="13.9" customHeight="1" s="3">
@@ -10664,8 +10694,11 @@
       <c r="KU11" s="2" t="n">
         <v>197</v>
       </c>
-      <c r="KV11" t="n">
+      <c r="KV11" s="2" t="n">
         <v>162</v>
+      </c>
+      <c r="KW11" t="n">
+        <v>238</v>
       </c>
     </row>
     <row r="12" ht="13.9" customHeight="1" s="3">
@@ -11592,8 +11625,11 @@
       <c r="KU12" s="2" t="n">
         <v>99</v>
       </c>
-      <c r="KV12" t="n">
+      <c r="KV12" s="2" t="n">
         <v>102</v>
+      </c>
+      <c r="KW12" t="n">
+        <v>100</v>
       </c>
     </row>
     <row r="13" ht="13.9" customHeight="1" s="3">
@@ -12520,8 +12556,11 @@
       <c r="KU13" s="2" t="n">
         <v>296</v>
       </c>
-      <c r="KV13" t="n">
+      <c r="KV13" s="2" t="n">
         <v>264</v>
+      </c>
+      <c r="KW13" t="n">
+        <v>338</v>
       </c>
     </row>
     <row r="14" ht="13.9" customHeight="1" s="3">
@@ -13448,8 +13487,11 @@
       <c r="KU14" s="2" t="n">
         <v>1.99</v>
       </c>
-      <c r="KV14" t="n">
+      <c r="KV14" s="2" t="n">
         <v>1.59</v>
+      </c>
+      <c r="KW14" t="n">
+        <v>2.38</v>
       </c>
     </row>
     <row r="15" ht="13.9" customHeight="1" s="3">
@@ -14376,8 +14418,11 @@
       <c r="KU15" s="2" t="n">
         <v>88</v>
       </c>
-      <c r="KV15" t="n">
+      <c r="KV15" s="2" t="n">
         <v>52</v>
+      </c>
+      <c r="KW15" t="n">
+        <v>92</v>
       </c>
     </row>
     <row r="16" ht="13.9" customHeight="1" s="3">
@@ -15304,8 +15349,11 @@
       <c r="KU16" s="2" t="n">
         <v>68</v>
       </c>
-      <c r="KV16" t="n">
+      <c r="KV16" s="2" t="n">
         <v>46</v>
+      </c>
+      <c r="KW16" t="n">
+        <v>49</v>
       </c>
     </row>
     <row r="17" ht="13.9" customHeight="1" s="3">
@@ -16232,8 +16280,11 @@
       <c r="KU17" s="2" t="n">
         <v>41</v>
       </c>
-      <c r="KV17" t="n">
+      <c r="KV17" s="2" t="n">
         <v>41</v>
+      </c>
+      <c r="KW17" t="n">
+        <v>43</v>
       </c>
     </row>
     <row r="18" ht="13.9" customHeight="1" s="3">
@@ -17160,8 +17211,11 @@
       <c r="KU18" s="2" t="n">
         <v>22</v>
       </c>
-      <c r="KV18" t="n">
+      <c r="KV18" s="2" t="n">
         <v>25</v>
+      </c>
+      <c r="KW18" t="n">
+        <v>18</v>
       </c>
     </row>
     <row r="19" ht="13.9" customHeight="1" s="3">
@@ -18088,8 +18142,11 @@
       <c r="KU19" s="2" t="n">
         <v>13</v>
       </c>
-      <c r="KV19" t="n">
+      <c r="KV19" s="2" t="n">
         <v>12</v>
+      </c>
+      <c r="KW19" t="n">
+        <v>17</v>
       </c>
     </row>
     <row r="20" ht="13.9" customHeight="1" s="3">
@@ -19016,8 +19073,11 @@
       <c r="KU20" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="KV20" t="n">
+      <c r="KV20" s="2" t="n">
         <v>11</v>
+      </c>
+      <c r="KW20" t="n">
+        <v>14</v>
       </c>
     </row>
     <row r="21" ht="13.9" customHeight="1" s="3">
@@ -19944,8 +20004,11 @@
       <c r="KU21" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="KV21" t="n">
+      <c r="KV21" s="2" t="n">
         <v>4</v>
+      </c>
+      <c r="KW21" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="22" ht="13.9" customHeight="1" s="3">
@@ -20872,8 +20935,11 @@
       <c r="KU22" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="KV22" t="n">
+      <c r="KV22" s="2" t="n">
         <v>3</v>
+      </c>
+      <c r="KW22" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="23" ht="13.9" customHeight="1" s="3">
@@ -21800,8 +21866,11 @@
       <c r="KU23" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="KV23" t="n">
+      <c r="KV23" s="2" t="n">
         <v>3</v>
+      </c>
+      <c r="KW23" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="24" ht="13.9" customHeight="1" s="3">
@@ -22728,8 +22797,11 @@
       <c r="KU24" s="2" t="n">
         <v>14</v>
       </c>
-      <c r="KV24" t="n">
+      <c r="KV24" s="2" t="n">
         <v>17</v>
+      </c>
+      <c r="KW24" t="n">
+        <v>23</v>
       </c>
     </row>
     <row r="25" ht="13.9" customHeight="1" s="3">
@@ -23656,8 +23728,11 @@
       <c r="KU25" s="2" t="n">
         <v>50</v>
       </c>
-      <c r="KV25" t="n">
+      <c r="KV25" s="2" t="n">
         <v>64.7</v>
+      </c>
+      <c r="KW25" t="n">
+        <v>60.9</v>
       </c>
     </row>
     <row r="26" ht="13.9" customHeight="1" s="3">
@@ -24584,8 +24659,11 @@
       <c r="KU26" s="2" t="n">
         <v>42.29</v>
       </c>
-      <c r="KV26" t="n">
+      <c r="KV26" s="2" t="n">
         <v>24</v>
+      </c>
+      <c r="KW26" t="n">
+        <v>24.14</v>
       </c>
     </row>
     <row r="27" ht="13.9" customHeight="1" s="3">
@@ -25512,8 +25590,11 @@
       <c r="KU27" s="2" t="n">
         <v>21.14</v>
       </c>
-      <c r="KV27" t="n">
+      <c r="KV27" s="2" t="n">
         <v>15.53</v>
+      </c>
+      <c r="KW27" t="n">
+        <v>14.7</v>
       </c>
     </row>
     <row r="28" ht="13.9" customHeight="1" s="3">
@@ -26440,8 +26521,11 @@
       <c r="KU28" s="2" t="n">
         <v>40</v>
       </c>
-      <c r="KV28" t="n">
+      <c r="KV28" s="2" t="n">
         <v>38</v>
+      </c>
+      <c r="KW28" t="n">
+        <v>60</v>
       </c>
     </row>
     <row r="29" ht="13.9" customHeight="1" s="3">
@@ -27368,8 +27452,11 @@
       <c r="KU29" s="2" t="n">
         <v>50</v>
       </c>
-      <c r="KV29" t="n">
+      <c r="KV29" s="2" t="n">
         <v>48</v>
+      </c>
+      <c r="KW29" t="n">
+        <v>69</v>
       </c>
     </row>
     <row r="30" ht="13.9" customHeight="1" s="3">
@@ -28296,8 +28383,11 @@
       <c r="KU30" s="2" t="n">
         <v>41</v>
       </c>
-      <c r="KV30" t="n">
+      <c r="KV30" s="2" t="n">
         <v>47</v>
+      </c>
+      <c r="KW30" t="n">
+        <v>39</v>
       </c>
     </row>
     <row r="31" ht="13.9" customHeight="1" s="3">
@@ -29224,8 +29314,11 @@
       <c r="KU31" s="2" t="n">
         <v>46</v>
       </c>
-      <c r="KV31" t="n">
+      <c r="KV31" s="2" t="n">
         <v>40</v>
+      </c>
+      <c r="KW31" t="n">
+        <v>59</v>
       </c>
     </row>
     <row r="32" ht="13.9" customHeight="1" s="3">
@@ -30152,8 +30245,11 @@
       <c r="KU32" s="2" t="n">
         <v>3.29</v>
       </c>
-      <c r="KV32" t="n">
+      <c r="KV32" s="2" t="n">
         <v>2.35</v>
+      </c>
+      <c r="KW32" t="n">
+        <v>2.57</v>
       </c>
     </row>
     <row r="33" ht="13.9" customHeight="1" s="3">
@@ -31080,8 +31176,11 @@
       <c r="KU33" s="2" t="n">
         <v>6.57</v>
       </c>
-      <c r="KV33" t="n">
+      <c r="KV33" s="2" t="n">
         <v>3.64</v>
+      </c>
+      <c r="KW33" t="n">
+        <v>4.21</v>
       </c>
     </row>
     <row r="34" ht="13.9" customHeight="1" s="3">
@@ -32008,8 +32107,11 @@
       <c r="KU34" s="2" t="n">
         <v>30.4</v>
       </c>
-      <c r="KV34" t="n">
+      <c r="KV34" s="2" t="n">
         <v>35</v>
+      </c>
+      <c r="KW34" t="n">
+        <v>35.6</v>
       </c>
     </row>
     <row r="35" ht="13.9" customHeight="1" s="3">
@@ -32936,8 +33038,11 @@
       <c r="KU35" s="2" t="n">
         <v>15.2</v>
       </c>
-      <c r="KV35" t="n">
+      <c r="KV35" s="2" t="n">
         <v>27.5</v>
+      </c>
+      <c r="KW35" t="n">
+        <v>23.7</v>
       </c>
     </row>
     <row r="36" ht="13.9" customHeight="1" s="3">
@@ -33864,8 +33969,11 @@
       <c r="KU36" s="2" t="n">
         <v>187.9</v>
       </c>
-      <c r="KV36" t="n">
+      <c r="KV36" s="2" t="n">
         <v>188.4</v>
+      </c>
+      <c r="KW36" t="n">
+        <v>189.1</v>
       </c>
     </row>
     <row r="37" ht="13.9" customHeight="1" s="3">
@@ -34792,8 +34900,11 @@
       <c r="KU37" s="2" t="n">
         <v>87.8</v>
       </c>
-      <c r="KV37" t="n">
+      <c r="KV37" s="2" t="n">
         <v>88.3</v>
+      </c>
+      <c r="KW37" t="n">
+        <v>89.8</v>
       </c>
     </row>
     <row r="38" ht="13.9" customHeight="1" s="3">
@@ -35720,8 +35831,11 @@
       <c r="KU38" s="2" t="n">
         <v>25.66</v>
       </c>
-      <c r="KV38" t="n">
+      <c r="KV38" s="2" t="n">
         <v>25.33</v>
+      </c>
+      <c r="KW38" t="n">
+        <v>26.49</v>
       </c>
     </row>
     <row r="39" ht="13.9" customHeight="1" s="3">
@@ -36648,8 +36762,11 @@
       <c r="KU39" s="2" t="n">
         <v>116.6</v>
       </c>
-      <c r="KV39" t="n">
+      <c r="KV39" s="2" t="n">
         <v>103.7</v>
+      </c>
+      <c r="KW39" t="n">
+        <v>113</v>
       </c>
     </row>
     <row r="40" ht="13.9" customHeight="1" s="3">
@@ -37576,8 +37693,11 @@
       <c r="KU40" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="KV40" t="n">
+      <c r="KV40" s="2" t="n">
         <v>7</v>
+      </c>
+      <c r="KW40" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="41" ht="13.9" customHeight="1" s="3">
@@ -38504,7 +38624,10 @@
       <c r="KU41" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="KV41" t="n">
+      <c r="KV41" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="KW41" t="n">
         <v>4</v>
       </c>
     </row>
@@ -39432,7 +39555,10 @@
       <c r="KU42" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="KV42" t="n">
+      <c r="KV42" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="KW42" t="n">
         <v>6</v>
       </c>
     </row>
@@ -40360,8 +40486,11 @@
       <c r="KU43" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="KV43" t="n">
+      <c r="KV43" s="2" t="n">
         <v>6</v>
+      </c>
+      <c r="KW43" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="44" ht="13.9" customHeight="1" s="3">
@@ -41288,8 +41417,11 @@
       <c r="KU44" s="2" t="n">
         <v>117</v>
       </c>
-      <c r="KV44" t="n">
+      <c r="KV44" s="2" t="n">
         <v>116</v>
+      </c>
+      <c r="KW44" t="n">
+        <v>151</v>
       </c>
     </row>
     <row r="45" ht="13.9" customHeight="1" s="3">
@@ -42216,8 +42348,11 @@
       <c r="KU45" s="2" t="n">
         <v>177</v>
       </c>
-      <c r="KV45" t="n">
+      <c r="KV45" s="2" t="n">
         <v>130</v>
+      </c>
+      <c r="KW45" t="n">
+        <v>184</v>
       </c>
     </row>
     <row r="46" ht="13.9" customHeight="1" s="3">
@@ -43144,8 +43279,11 @@
       <c r="KU46" s="2" t="n">
         <v>200</v>
       </c>
-      <c r="KV46" t="n">
+      <c r="KV46" s="2" t="n">
         <v>181</v>
+      </c>
+      <c r="KW46" t="n">
+        <v>234</v>
       </c>
     </row>
     <row r="47" ht="13.9" customHeight="1" s="3">
@@ -44072,8 +44210,11 @@
       <c r="KU47" s="2" t="n">
         <v>67.59999999999999</v>
       </c>
-      <c r="KV47" t="n">
+      <c r="KV47" s="2" t="n">
         <v>68.59999999999999</v>
+      </c>
+      <c r="KW47" t="n">
+        <v>69.2</v>
       </c>
     </row>
     <row r="48" ht="13.9" customHeight="1" s="3">
@@ -45000,8 +45141,11 @@
       <c r="KU48" s="2" t="n">
         <v>50</v>
       </c>
-      <c r="KV48" t="n">
+      <c r="KV48" s="2" t="n">
         <v>48</v>
+      </c>
+      <c r="KW48" t="n">
+        <v>69</v>
       </c>
     </row>
     <row r="49" ht="13.9" customHeight="1" s="3">
@@ -45928,8 +46072,11 @@
       <c r="KU49" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="KV49" t="n">
+      <c r="KV49" s="2" t="n">
         <v>4</v>
+      </c>
+      <c r="KW49" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="50" ht="13.9" customHeight="1" s="3">
@@ -46856,8 +47003,11 @@
       <c r="KU50" s="2" t="n">
         <v>11</v>
       </c>
-      <c r="KV50" t="n">
+      <c r="KV50" s="2" t="n">
         <v>6</v>
+      </c>
+      <c r="KW50" t="n">
+        <v>12</v>
       </c>
     </row>
     <row r="51" ht="13.9" customHeight="1" s="3">
@@ -47784,8 +47934,11 @@
       <c r="KU51" s="2" t="n">
         <v>40</v>
       </c>
-      <c r="KV51" t="n">
+      <c r="KV51" s="2" t="n">
         <v>38</v>
+      </c>
+      <c r="KW51" t="n">
+        <v>60</v>
       </c>
     </row>
     <row r="52" ht="13.9" customHeight="1" s="3">
@@ -48712,8 +48865,11 @@
       <c r="KU52" s="2" t="n">
         <v>41</v>
       </c>
-      <c r="KV52" t="n">
+      <c r="KV52" s="2" t="n">
         <v>47</v>
+      </c>
+      <c r="KW52" t="n">
+        <v>39</v>
       </c>
     </row>
     <row r="53" ht="13.9" customHeight="1" s="3">
@@ -49640,8 +49796,11 @@
       <c r="KU53" s="2" t="n">
         <v>37</v>
       </c>
-      <c r="KV53" t="n">
+      <c r="KV53" s="2" t="n">
         <v>45</v>
+      </c>
+      <c r="KW53" t="n">
+        <v>56</v>
       </c>
     </row>
     <row r="54" ht="13.9" customHeight="1" s="3">
@@ -50568,7 +50727,10 @@
       <c r="KU54" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="KV54" t="n">
+      <c r="KV54" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="KW54" t="n">
         <v>1</v>
       </c>
     </row>
@@ -51496,8 +51658,11 @@
       <c r="KU55" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="KV55" t="n">
+      <c r="KV55" s="2" t="n">
         <v>4</v>
+      </c>
+      <c r="KW55" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="56" ht="13.9" customHeight="1" s="3">
@@ -52424,8 +52589,11 @@
       <c r="KU56" s="2" t="n">
         <v>100</v>
       </c>
-      <c r="KV56" t="n">
+      <c r="KV56" s="2" t="n">
         <v>36.4</v>
+      </c>
+      <c r="KW56" t="n">
+        <v>71.40000000000001</v>
       </c>
     </row>
     <row r="57" ht="13.9" customHeight="1" s="3">
@@ -53352,8 +53520,11 @@
       <c r="KU57" s="2" t="n">
         <v>209</v>
       </c>
-      <c r="KV57" t="n">
+      <c r="KV57" s="2" t="n">
         <v>230</v>
+      </c>
+      <c r="KW57" t="n">
+        <v>201</v>
       </c>
     </row>
     <row r="58" ht="13.9" customHeight="1" s="3">
@@ -54280,8 +54451,11 @@
       <c r="KU58" s="2" t="n">
         <v>152</v>
       </c>
-      <c r="KV58" t="n">
+      <c r="KV58" s="2" t="n">
         <v>175</v>
+      </c>
+      <c r="KW58" t="n">
+        <v>149</v>
       </c>
     </row>
     <row r="59" ht="13.9" customHeight="1" s="3">
@@ -55208,8 +55382,11 @@
       <c r="KU59" s="2" t="n">
         <v>361</v>
       </c>
-      <c r="KV59" t="n">
+      <c r="KV59" s="2" t="n">
         <v>405</v>
+      </c>
+      <c r="KW59" t="n">
+        <v>350</v>
       </c>
     </row>
     <row r="60" ht="13.9" customHeight="1" s="3">
@@ -56136,8 +56313,11 @@
       <c r="KU60" s="2" t="n">
         <v>1.38</v>
       </c>
-      <c r="KV60" t="n">
+      <c r="KV60" s="2" t="n">
         <v>1.31</v>
+      </c>
+      <c r="KW60" t="n">
+        <v>1.35</v>
       </c>
     </row>
     <row r="61" ht="13.9" customHeight="1" s="3">
@@ -57064,8 +57244,11 @@
       <c r="KU61" s="2" t="n">
         <v>102</v>
       </c>
-      <c r="KV61" t="n">
+      <c r="KV61" s="2" t="n">
         <v>111</v>
+      </c>
+      <c r="KW61" t="n">
+        <v>69</v>
       </c>
     </row>
     <row r="62" ht="13.9" customHeight="1" s="3">
@@ -57992,8 +58175,11 @@
       <c r="KU62" s="2" t="n">
         <v>65</v>
       </c>
-      <c r="KV62" t="n">
+      <c r="KV62" s="2" t="n">
         <v>44</v>
+      </c>
+      <c r="KW62" t="n">
+        <v>66</v>
       </c>
     </row>
     <row r="63" ht="13.9" customHeight="1" s="3">
@@ -58920,8 +59106,11 @@
       <c r="KU63" s="2" t="n">
         <v>41</v>
       </c>
-      <c r="KV63" t="n">
+      <c r="KV63" s="2" t="n">
         <v>39</v>
+      </c>
+      <c r="KW63" t="n">
+        <v>52</v>
       </c>
     </row>
     <row r="64" ht="13.9" customHeight="1" s="3">
@@ -59848,8 +60037,11 @@
       <c r="KU64" s="2" t="n">
         <v>13</v>
       </c>
-      <c r="KV64" t="n">
+      <c r="KV64" s="2" t="n">
         <v>12</v>
+      </c>
+      <c r="KW64" t="n">
+        <v>17</v>
       </c>
     </row>
     <row r="65" ht="13.9" customHeight="1" s="3">
@@ -60776,8 +60968,11 @@
       <c r="KU65" s="2" t="n">
         <v>22</v>
       </c>
-      <c r="KV65" t="n">
+      <c r="KV65" s="2" t="n">
         <v>25</v>
+      </c>
+      <c r="KW65" t="n">
+        <v>18</v>
       </c>
     </row>
     <row r="66" ht="13.9" customHeight="1" s="3">
@@ -61704,8 +61899,11 @@
       <c r="KU66" s="2" t="n">
         <v>18</v>
       </c>
-      <c r="KV66" t="n">
+      <c r="KV66" s="2" t="n">
         <v>18</v>
+      </c>
+      <c r="KW66" t="n">
+        <v>13</v>
       </c>
     </row>
     <row r="67" ht="13.9" customHeight="1" s="3">
@@ -62632,8 +62830,11 @@
       <c r="KU67" s="2" t="n">
         <v>14</v>
       </c>
-      <c r="KV67" t="n">
+      <c r="KV67" s="2" t="n">
         <v>14</v>
+      </c>
+      <c r="KW67" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="68" ht="13.9" customHeight="1" s="3">
@@ -63560,8 +63761,11 @@
       <c r="KU68" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="KV68" t="n">
+      <c r="KV68" s="2" t="n">
         <v>16</v>
+      </c>
+      <c r="KW68" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="69" ht="13.9" customHeight="1" s="3">
@@ -64488,8 +64692,11 @@
       <c r="KU69" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="KV69" t="n">
+      <c r="KV69" s="2" t="n">
         <v>2</v>
+      </c>
+      <c r="KW69" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="70" ht="13.9" customHeight="1" s="3">
@@ -65416,8 +65623,11 @@
       <c r="KU70" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="KV70" t="n">
+      <c r="KV70" s="2" t="n">
         <v>36</v>
+      </c>
+      <c r="KW70" t="n">
+        <v>17</v>
       </c>
     </row>
     <row r="71" ht="13.9" customHeight="1" s="3">
@@ -66344,8 +66554,11 @@
       <c r="KU71" s="2" t="n">
         <v>60</v>
       </c>
-      <c r="KV71" t="n">
+      <c r="KV71" s="2" t="n">
         <v>50</v>
+      </c>
+      <c r="KW71" t="n">
+        <v>76.5</v>
       </c>
     </row>
     <row r="72" ht="13.9" customHeight="1" s="3">
@@ -67272,8 +67485,11 @@
       <c r="KU72" s="2" t="n">
         <v>20.06</v>
       </c>
-      <c r="KV72" t="n">
+      <c r="KV72" s="2" t="n">
         <v>22.5</v>
+      </c>
+      <c r="KW72" t="n">
+        <v>26.92</v>
       </c>
     </row>
     <row r="73" ht="13.9" customHeight="1" s="3">
@@ -68200,8 +68416,11 @@
       <c r="KU73" s="2" t="n">
         <v>12.03</v>
       </c>
-      <c r="KV73" t="n">
+      <c r="KV73" s="2" t="n">
         <v>11.25</v>
+      </c>
+      <c r="KW73" t="n">
+        <v>20.59</v>
       </c>
     </row>
     <row r="74" ht="13.9" customHeight="1" s="3">
@@ -69128,8 +69347,11 @@
       <c r="KU74" s="2" t="n">
         <v>37</v>
       </c>
-      <c r="KV74" t="n">
+      <c r="KV74" s="2" t="n">
         <v>47</v>
+      </c>
+      <c r="KW74" t="n">
+        <v>32</v>
       </c>
     </row>
     <row r="75" ht="13.9" customHeight="1" s="3">
@@ -70056,8 +70278,11 @@
       <c r="KU75" s="2" t="n">
         <v>55</v>
       </c>
-      <c r="KV75" t="n">
+      <c r="KV75" s="2" t="n">
         <v>55</v>
+      </c>
+      <c r="KW75" t="n">
+        <v>57</v>
       </c>
     </row>
     <row r="76" ht="13.9" customHeight="1" s="3">
@@ -70984,8 +71209,11 @@
       <c r="KU76" s="2" t="n">
         <v>38</v>
       </c>
-      <c r="KV76" t="n">
+      <c r="KV76" s="2" t="n">
         <v>29</v>
+      </c>
+      <c r="KW76" t="n">
+        <v>44</v>
       </c>
     </row>
     <row r="77" ht="13.9" customHeight="1" s="3">
@@ -71912,8 +72140,11 @@
       <c r="KU77" s="2" t="n">
         <v>59</v>
       </c>
-      <c r="KV77" t="n">
+      <c r="KV77" s="2" t="n">
         <v>65</v>
+      </c>
+      <c r="KW77" t="n">
+        <v>54</v>
       </c>
     </row>
     <row r="78" ht="13.9" customHeight="1" s="3">
@@ -72840,8 +73071,11 @@
       <c r="KU78" s="2" t="n">
         <v>1.97</v>
       </c>
-      <c r="KV78" t="n">
+      <c r="KV78" s="2" t="n">
         <v>1.81</v>
+      </c>
+      <c r="KW78" t="n">
+        <v>3.18</v>
       </c>
     </row>
     <row r="79" ht="13.9" customHeight="1" s="3">
@@ -73768,8 +74002,11 @@
       <c r="KU79" s="2" t="n">
         <v>3.28</v>
       </c>
-      <c r="KV79" t="n">
+      <c r="KV79" s="2" t="n">
         <v>3.61</v>
+      </c>
+      <c r="KW79" t="n">
+        <v>4.15</v>
       </c>
     </row>
     <row r="80" ht="13.9" customHeight="1" s="3">
@@ -74696,8 +74933,11 @@
       <c r="KU80" s="2" t="n">
         <v>47.5</v>
       </c>
-      <c r="KV80" t="n">
+      <c r="KV80" s="2" t="n">
         <v>52.3</v>
+      </c>
+      <c r="KW80" t="n">
+        <v>29.6</v>
       </c>
     </row>
     <row r="81" ht="13.9" customHeight="1" s="3">
@@ -75624,8 +75864,11 @@
       <c r="KU81" s="2" t="n">
         <v>30.5</v>
       </c>
-      <c r="KV81" t="n">
+      <c r="KV81" s="2" t="n">
         <v>27.7</v>
+      </c>
+      <c r="KW81" t="n">
+        <v>24.1</v>
       </c>
     </row>
     <row r="82" ht="13.9" customHeight="1" s="3">
@@ -76552,8 +76795,11 @@
       <c r="KU82" s="2" t="n">
         <v>188.9</v>
       </c>
-      <c r="KV82" t="n">
+      <c r="KV82" s="2" t="n">
         <v>187.7</v>
+      </c>
+      <c r="KW82" t="n">
+        <v>187.9</v>
       </c>
     </row>
     <row r="83" ht="13.9" customHeight="1" s="3">
@@ -77480,8 +77726,11 @@
       <c r="KU83" s="2" t="n">
         <v>88</v>
       </c>
-      <c r="KV83" t="n">
+      <c r="KV83" s="2" t="n">
         <v>87.3</v>
+      </c>
+      <c r="KW83" t="n">
+        <v>88.09999999999999</v>
       </c>
     </row>
     <row r="84" ht="13.9" customHeight="1" s="3">
@@ -78408,8 +78657,11 @@
       <c r="KU84" s="2" t="n">
         <v>28.33</v>
       </c>
-      <c r="KV84" t="n">
+      <c r="KV84" s="2" t="n">
         <v>25.66</v>
+      </c>
+      <c r="KW84" t="n">
+        <v>26.49</v>
       </c>
     </row>
     <row r="85" ht="13.9" customHeight="1" s="3">
@@ -79336,8 +79588,11 @@
       <c r="KU85" s="2" t="n">
         <v>163.1</v>
       </c>
-      <c r="KV85" t="n">
+      <c r="KV85" s="2" t="n">
         <v>94</v>
+      </c>
+      <c r="KW85" t="n">
+        <v>123.7</v>
       </c>
     </row>
     <row r="86" ht="13.9" customHeight="1" s="3">
@@ -80264,8 +80519,11 @@
       <c r="KU86" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="KV86" t="n">
+      <c r="KV86" s="2" t="n">
         <v>5</v>
+      </c>
+      <c r="KW86" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="87" ht="13.9" customHeight="1" s="3">
@@ -81192,8 +81450,11 @@
       <c r="KU87" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="KV87" t="n">
+      <c r="KV87" s="2" t="n">
         <v>8</v>
+      </c>
+      <c r="KW87" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="88" ht="13.9" customHeight="1" s="3">
@@ -82120,8 +82381,11 @@
       <c r="KU88" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="KV88" t="n">
+      <c r="KV88" s="2" t="n">
         <v>6</v>
+      </c>
+      <c r="KW88" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="89" ht="13.9" customHeight="1" s="3">
@@ -83048,8 +83312,11 @@
       <c r="KU89" s="2" t="n">
         <v>13</v>
       </c>
-      <c r="KV89" t="n">
+      <c r="KV89" s="2" t="n">
         <v>4</v>
+      </c>
+      <c r="KW89" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="90" ht="13.9" customHeight="1" s="3">
@@ -83976,8 +84243,11 @@
       <c r="KU90" s="2" t="n">
         <v>125</v>
       </c>
-      <c r="KV90" t="n">
+      <c r="KV90" s="2" t="n">
         <v>150</v>
+      </c>
+      <c r="KW90" t="n">
+        <v>136</v>
       </c>
     </row>
     <row r="91" ht="13.9" customHeight="1" s="3">
@@ -84904,8 +85174,11 @@
       <c r="KU91" s="2" t="n">
         <v>230</v>
       </c>
-      <c r="KV91" t="n">
+      <c r="KV91" s="2" t="n">
         <v>257</v>
+      </c>
+      <c r="KW91" t="n">
+        <v>200</v>
       </c>
     </row>
     <row r="92" ht="13.9" customHeight="1" s="3">
@@ -85832,8 +86105,11 @@
       <c r="KU92" s="2" t="n">
         <v>274</v>
       </c>
-      <c r="KV92" t="n">
+      <c r="KV92" s="2" t="n">
         <v>300</v>
+      </c>
+      <c r="KW92" t="n">
+        <v>249</v>
       </c>
     </row>
     <row r="93" ht="13.9" customHeight="1" s="3">
@@ -86760,8 +87036,11 @@
       <c r="KU93" s="2" t="n">
         <v>75.90000000000001</v>
       </c>
-      <c r="KV93" t="n">
+      <c r="KV93" s="2" t="n">
         <v>74.09999999999999</v>
+      </c>
+      <c r="KW93" t="n">
+        <v>71.09999999999999</v>
       </c>
     </row>
     <row r="94" ht="13.9" customHeight="1" s="3">
@@ -87688,8 +87967,11 @@
       <c r="KU94" s="2" t="n">
         <v>55</v>
       </c>
-      <c r="KV94" t="n">
+      <c r="KV94" s="2" t="n">
         <v>55</v>
+      </c>
+      <c r="KW94" t="n">
+        <v>57</v>
       </c>
     </row>
     <row r="95" ht="13.9" customHeight="1" s="3">
@@ -88616,8 +88898,11 @@
       <c r="KU95" s="2" t="n">
         <v>15</v>
       </c>
-      <c r="KV95" t="n">
+      <c r="KV95" s="2" t="n">
         <v>19</v>
+      </c>
+      <c r="KW95" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="96" ht="13.9" customHeight="1" s="3">
@@ -89544,8 +89829,11 @@
       <c r="KU96" s="2" t="n">
         <v>15</v>
       </c>
-      <c r="KV96" t="n">
+      <c r="KV96" s="2" t="n">
         <v>24</v>
+      </c>
+      <c r="KW96" t="n">
+        <v>11</v>
       </c>
     </row>
     <row r="97" ht="13.9" customHeight="1" s="3">
@@ -90472,8 +90760,11 @@
       <c r="KU97" s="2" t="n">
         <v>37</v>
       </c>
-      <c r="KV97" t="n">
+      <c r="KV97" s="2" t="n">
         <v>47</v>
+      </c>
+      <c r="KW97" t="n">
+        <v>32</v>
       </c>
     </row>
     <row r="98" ht="13.9" customHeight="1" s="3">
@@ -91400,8 +91691,11 @@
       <c r="KU98" s="2" t="n">
         <v>38</v>
       </c>
-      <c r="KV98" t="n">
+      <c r="KV98" s="2" t="n">
         <v>29</v>
+      </c>
+      <c r="KW98" t="n">
+        <v>44</v>
       </c>
     </row>
     <row r="99" ht="13.9" customHeight="1" s="3">
@@ -92328,8 +92622,11 @@
       <c r="KU99" s="2" t="n">
         <v>48</v>
       </c>
-      <c r="KV99" t="n">
+      <c r="KV99" s="2" t="n">
         <v>46</v>
+      </c>
+      <c r="KW99" t="n">
+        <v>41</v>
       </c>
     </row>
     <row r="100" ht="13.9" customHeight="1" s="3">
@@ -93256,8 +93553,11 @@
       <c r="KU100" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="KV100" t="n">
+      <c r="KV100" s="2" t="n">
         <v>5</v>
+      </c>
+      <c r="KW100" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="101" ht="13.9" customHeight="1" s="3">
@@ -94184,8 +94484,11 @@
       <c r="KU101" s="2" t="n">
         <v>14</v>
       </c>
-      <c r="KV101" t="n">
+      <c r="KV101" s="2" t="n">
         <v>14</v>
+      </c>
+      <c r="KW101" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="102" ht="13.9" customHeight="1" s="3">
@@ -95112,8 +95415,11 @@
       <c r="KU102" s="2" t="n">
         <v>77.8</v>
       </c>
-      <c r="KV102" t="n">
+      <c r="KV102" s="2" t="n">
         <v>77.8</v>
+      </c>
+      <c r="KW102" t="n">
+        <v>69.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>